<commit_message>
se le agregó funcion para que lea xlsx y xls.
</commit_message>
<xml_diff>
--- a/diferentes_tipos de celdas.xlsx
+++ b/diferentes_tipos de celdas.xlsx
@@ -139,7 +139,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>43047.692215752315</v>
+        <v>43053.559834328706</v>
       </c>
     </row>
     <row r="8">
@@ -153,7 +153,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n" s="1">
-        <v>43047.692215902774</v>
+        <v>43053.559834479165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entrando a correo de empresa
</commit_message>
<xml_diff>
--- a/diferentes_tipos de celdas.xlsx
+++ b/diferentes_tipos de celdas.xlsx
@@ -139,7 +139,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>43053.559834328706</v>
+        <v>43055.765722233795</v>
       </c>
     </row>
     <row r="8">
@@ -153,7 +153,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n" s="1">
-        <v>43053.559834479165</v>
+        <v>43055.76572238426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>